<commit_message>
tipoIdentifier, codesystem 0203, conselhos profissionais
</commit_message>
<xml_diff>
--- a/Entregaveis/1.RepositorioSemantico/Pacientes/TipoIdentifier.xlsx
+++ b/Entregaveis/1.RepositorioSemantico/Pacientes/TipoIdentifier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beatrizdefarialeao/Documents/GitHub/ips-brasil-documentos/Entregaveis/1.RepositorioSemantico/Pacientes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C960D463-0DC8-8448-988F-53ABDB38E5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3EC1B5-61E2-5A4A-9123-DCA6AED228B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{F1A188C6-0B5E-AD40-B3C6-40C868E7058F}"/>
+    <workbookView xWindow="1440" yWindow="760" windowWidth="27240" windowHeight="16440" xr2:uid="{F1A188C6-0B5E-AD40-B3C6-40C868E7058F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
   <si>
     <t>Code</t>
   </si>
@@ -228,6 +228,42 @@
   </si>
   <si>
     <t>Naming systems de acordo com GI IPS.</t>
+  </si>
+  <si>
+    <t>Número do Microchip</t>
+  </si>
+  <si>
+    <t>Número do Empregador</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Identificação do Profissional</t>
+  </si>
+  <si>
+    <t>Número de Registro de Doador</t>
+  </si>
+  <si>
+    <t>Idenfificador Universal do Dispositivo</t>
+  </si>
+  <si>
+    <t>Número de Série</t>
+  </si>
+  <si>
+    <t>Identificador do Seguro Nacional</t>
+  </si>
+  <si>
+    <t>Identificador do Beneficiário Social</t>
+  </si>
+  <si>
+    <t>Identifcador do Placer</t>
+  </si>
+  <si>
+    <t>Identificador do Filler</t>
+  </si>
+  <si>
+    <t>Identificador Provincial de Saúde (Canada)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +340,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -318,15 +360,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -645,7 +689,7 @@
   <dimension ref="A2:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B24" sqref="B24:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,14 +793,16 @@
       <c r="K6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="Q6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -768,7 +814,9 @@
       <c r="K7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="Q7" s="2" t="s">
         <v>36</v>
       </c>
@@ -787,7 +835,9 @@
       <c r="K8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="Q8" s="2" t="s">
         <v>38</v>
       </c>
@@ -806,7 +856,9 @@
       <c r="K9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="Q9" s="2" t="s">
         <v>28</v>
       </c>
@@ -822,17 +874,19 @@
       <c r="J10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="Q10" s="2" t="s">
         <v>41</v>
       </c>
       <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -845,14 +899,16 @@
       <c r="K11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="Q11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -864,14 +920,16 @@
       <c r="K12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="Q12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -883,7 +941,9 @@
       <c r="K13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="Q13" s="2" t="s">
         <v>46</v>
       </c>
@@ -899,7 +959,7 @@
       <c r="J14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="8" t="s">
         <v>49</v>
       </c>
       <c r="L14" s="5"/>
@@ -909,7 +969,7 @@
       <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -921,7 +981,9 @@
       <c r="K15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="Q15" s="2" t="s">
         <v>50</v>
       </c>
@@ -940,7 +1002,9 @@
       <c r="K16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="Q16" s="2" t="s">
         <v>52</v>
       </c>
@@ -953,7 +1017,9 @@
       <c r="K17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="Q17" s="2" t="s">
         <v>54</v>
       </c>
@@ -963,10 +1029,12 @@
       <c r="J18" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="Q18" s="2" t="s">
         <v>56</v>
       </c>
@@ -976,10 +1044,12 @@
       <c r="J19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="L19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="Q19" s="2" t="s">
         <v>58</v>
       </c>
@@ -992,6 +1062,10 @@
       <c r="K20" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="L20" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="M20" s="5"/>
       <c r="Q20" s="2" t="s">
         <v>60</v>
       </c>

</xml_diff>